<commit_message>
practice on Xlookup Horinzontal and Xlookup with SUM
</commit_message>
<xml_diff>
--- a/Excel/XLOOKUP Excel Tutorial File.xlsx
+++ b/Excel/XLOOKUP Excel Tutorial File.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\educa\Desktop\Udemy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\educa\Desktop\Udemy\Data-Analysis-Toolkit\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F15B10-36BD-4241-8818-C71A785576CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FDD20B-CC82-483F-8CF7-1E29F6BFE665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="12210" windowHeight="12885" firstSheet="3" activeTab="3" xr2:uid="{5EA44D8F-79D3-45F5-A0F6-C7F47358B7ED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="3" activeTab="5" xr2:uid="{5EA44D8F-79D3-45F5-A0F6-C7F47358B7ED}"/>
   </bookViews>
   <sheets>
     <sheet name="XLookUp" sheetId="1" r:id="rId1"/>
@@ -2005,7 +2005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22A42832-12A0-41C9-BED0-20D277223524}">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2414,7 +2414,7 @@
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2467,6 +2467,10 @@
       <c r="A2" t="s">
         <v>70</v>
       </c>
+      <c r="B2">
+        <f>_xlfn.XLOOKUP(B1,H1:S1,H2:S2)</f>
+        <v>310</v>
+      </c>
       <c r="G2" t="s">
         <v>70</v>
       </c>
@@ -2511,6 +2515,10 @@
       <c r="A3" t="s">
         <v>71</v>
       </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B4" si="0">_xlfn.XLOOKUP(B2,H2:S2,H3:S3)</f>
+        <v>40</v>
+      </c>
       <c r="G3" t="s">
         <v>71</v>
       </c>
@@ -2554,6 +2562,10 @@
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>84</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>118</v>
       </c>
       <c r="G4" t="s">
         <v>84</v>
@@ -2604,8 +2616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A2549A4-3A41-4806-B7FD-3B9C6823775F}">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2658,6 +2670,10 @@
       <c r="A2" t="s">
         <v>70</v>
       </c>
+      <c r="B2">
+        <f>_xlfn.XLOOKUP(B1,H1:S1,H2:S2)</f>
+        <v>310</v>
+      </c>
       <c r="G2" t="s">
         <v>70</v>
       </c>
@@ -2702,6 +2718,10 @@
       <c r="A3" t="s">
         <v>71</v>
       </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B4" si="0">_xlfn.XLOOKUP(B2,H2:S2,H3:S3)</f>
+        <v>40</v>
+      </c>
       <c r="G3" t="s">
         <v>71</v>
       </c>
@@ -2746,6 +2766,10 @@
       <c r="A4" t="s">
         <v>84</v>
       </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>118</v>
+      </c>
       <c r="G4" t="s">
         <v>84</v>
       </c>
@@ -2794,6 +2818,10 @@
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>70</v>
+      </c>
+      <c r="B7">
+        <f>SUM(_xlfn.XLOOKUP(I1,H1:S1,H2:S2):_xlfn.XLOOKUP(J1,H1:S1,H2:S2))</f>
+        <v>460</v>
       </c>
     </row>
   </sheetData>

</xml_diff>